<commit_message>
Added ECTS-grades to calc
</commit_message>
<xml_diff>
--- a/General_stuff/GradeaverageCalc.xlsx
+++ b/General_stuff/GradeaverageCalc.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorenmulvad/GoogleDrive/Uni/Generelt/DIKUNotes/General_stuff/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorenmulvad/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="-25600" yWindow="-10340" windowWidth="25600" windowHeight="28340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Gennemsnit" sheetId="1" r:id="rId1"/>
@@ -27,14 +27,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Fag</t>
   </si>
   <si>
-    <t>ECTS</t>
-  </si>
-  <si>
     <t>Karakter</t>
   </si>
   <si>
@@ -47,9 +44,6 @@
     <t>Vægtet karakter</t>
   </si>
   <si>
-    <t>Totale karaktervægte</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -86,15 +80,9 @@
     <t>Datalogiens videnskabsteori</t>
   </si>
   <si>
-    <t>ECTS-vægtet gennemsnit</t>
-  </si>
-  <si>
     <t>"Rent" gennemsnit</t>
   </si>
   <si>
-    <t>Totale ECTS-vægte</t>
-  </si>
-  <si>
     <t>Data Science</t>
   </si>
   <si>
@@ -102,6 +90,27 @@
   </si>
   <si>
     <t>Elements of Machine Learning</t>
+  </si>
+  <si>
+    <t>ECTS-point</t>
+  </si>
+  <si>
+    <t>ECTS-point vægtet gennemsnit</t>
+  </si>
+  <si>
+    <t>ECTS karakter</t>
+  </si>
+  <si>
+    <t>ECTS-vægtet karakter</t>
+  </si>
+  <si>
+    <t>Opnåede ECTS-point</t>
+  </si>
+  <si>
+    <t>"Rent" ECTS-gennemsnit</t>
+  </si>
+  <si>
+    <t>ECTS-point vægtet ECTS-gennemsnit</t>
   </si>
 </sst>
 </file>
@@ -181,32 +190,6 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -220,6 +203,32 @@
         <color auto="1"/>
       </right>
       <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom style="medium">
@@ -231,25 +240,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -264,14 +277,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FagTabel" displayName="FagTabel" ref="B1:E17" totalsRowShown="0">
-  <autoFilter ref="B1:E17"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FagTabel" displayName="FagTabel" ref="B1:G17" totalsRowShown="0">
+  <autoFilter ref="B1:G17"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="Fag"/>
-    <tableColumn id="2" name="ECTS"/>
+    <tableColumn id="2" name="ECTS-point"/>
     <tableColumn id="3" name="Karakter"/>
-    <tableColumn id="4" name="Vægtet karakter" dataDxfId="0">
-      <calculatedColumnFormula>IFERROR(FagTabel[[#This Row],[ECTS]]*FagTabel[[#This Row],[Karakter]], 0)</calculatedColumnFormula>
+    <tableColumn id="6" name="ECTS karakter" dataDxfId="2">
+      <calculatedColumnFormula>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]),IF(D2=12,4,IF(D2=10,3.3,IF(D2=7,3,IF(D2=4,2.3,IF(D2=2,2,IF(D2=0,0,IF(D2=-3,0,"Ukendt karakter"))))))), "")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Vægtet karakter" dataDxfId="1">
+      <calculatedColumnFormula>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]), FagTabel[[#This Row],[ECTS-point]]*FagTabel[[#This Row],[Karakter]],"")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="ECTS-vægtet karakter" dataDxfId="0">
+      <calculatedColumnFormula>IF(ISNUMBER(FagTabel[[#This Row],[ECTS karakter]]),FagTabel[[#This Row],[ECTS karakter]]*FagTabel[[#This Row],[ECTS-point]],"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -541,68 +560,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E22"/>
+  <dimension ref="B1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="169" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.5" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
-    <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="5" width="14.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="14" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
       <c r="E1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2">
-        <f>IFERROR(FagTabel[[#This Row],[ECTS]]*FagTabel[[#This Row],[Karakter]], 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="E2" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]),IF(D2=12,4,IF(D2=10,3.3,IF(D2=7,3,IF(D2=4,2.3,IF(D2=2,2,IF(D2=0,0,IF(D2=-3,0,"Ukendt karakter"))))))), "")</f>
+        <v/>
+      </c>
+      <c r="F2" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]), FagTabel[[#This Row],[ECTS-point]]*FagTabel[[#This Row],[Karakter]],"")</f>
+        <v/>
+      </c>
+      <c r="G2" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[ECTS karakter]]),FagTabel[[#This Row],[ECTS karakter]]*FagTabel[[#This Row],[ECTS-point]],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <f>IFERROR(FagTabel[[#This Row],[ECTS]]*FagTabel[[#This Row],[Karakter]], 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="E3" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]),IF(D3=12,4,IF(D3=10,3.3,IF(D3=7,3,IF(D3=4,2.3,IF(D3=2,2,IF(D3=0,0,IF(D3=-3,0,"Ukendt karakter"))))))), "")</f>
+        <v/>
+      </c>
+      <c r="F3" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]), FagTabel[[#This Row],[ECTS-point]]*FagTabel[[#This Row],[Karakter]],"")</f>
+        <v/>
+      </c>
+      <c r="G3" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[ECTS karakter]]),FagTabel[[#This Row],[ECTS karakter]]*FagTabel[[#This Row],[ECTS-point]],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>15</v>
@@ -611,13 +654,21 @@
         <v>2</v>
       </c>
       <c r="E4">
-        <f>IFERROR(FagTabel[[#This Row],[ECTS]]*FagTabel[[#This Row],[Karakter]], 0)</f>
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]),IF(D4=12,4,IF(D4=10,3.3,IF(D4=7,3,IF(D4=4,2.3,IF(D4=2,2,IF(D4=0,0,IF(D4=-3,0,"Ukendt karakter"))))))), "")</f>
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]), FagTabel[[#This Row],[ECTS-point]]*FagTabel[[#This Row],[Karakter]],"")</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[ECTS karakter]]),FagTabel[[#This Row],[ECTS karakter]]*FagTabel[[#This Row],[ECTS-point]],"")</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>7.5</v>
@@ -626,13 +677,21 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <f>IFERROR(FagTabel[[#This Row],[ECTS]]*FagTabel[[#This Row],[Karakter]], 0)</f>
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]),IF(D5=12,4,IF(D5=10,3.3,IF(D5=7,3,IF(D5=4,2.3,IF(D5=2,2,IF(D5=0,0,IF(D5=-3,0,"Ukendt karakter"))))))), "")</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F5">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]), FagTabel[[#This Row],[ECTS-point]]*FagTabel[[#This Row],[Karakter]],"")</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[ECTS karakter]]),FagTabel[[#This Row],[ECTS karakter]]*FagTabel[[#This Row],[ECTS-point]],"")</f>
+        <v>17.25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>7.5</v>
@@ -640,14 +699,22 @@
       <c r="D6">
         <v>7</v>
       </c>
-      <c r="E6" s="4">
-        <f>IFERROR(FagTabel[[#This Row],[ECTS]]*FagTabel[[#This Row],[Karakter]], 0)</f>
+      <c r="E6" s="2">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]),IF(D6=12,4,IF(D6=10,3.3,IF(D6=7,3,IF(D6=4,2.3,IF(D6=2,2,IF(D6=0,0,IF(D6=-3,0,"Ukendt karakter"))))))), "")</f>
+        <v>3</v>
+      </c>
+      <c r="F6" s="2">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]), FagTabel[[#This Row],[ECTS-point]]*FagTabel[[#This Row],[Karakter]],"")</f>
         <v>52.5</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[ECTS karakter]]),FagTabel[[#This Row],[ECTS karakter]]*FagTabel[[#This Row],[ECTS-point]],"")</f>
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>7.5</v>
@@ -655,166 +722,268 @@
       <c r="D7">
         <v>10</v>
       </c>
-      <c r="E7" s="4">
-        <f>IFERROR(FagTabel[[#This Row],[ECTS]]*FagTabel[[#This Row],[Karakter]], 0)</f>
+      <c r="E7" s="2">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]),IF(D7=12,4,IF(D7=10,3.3,IF(D7=7,3,IF(D7=4,2.3,IF(D7=2,2,IF(D7=0,0,IF(D7=-3,0,"Ukendt karakter"))))))), "")</f>
+        <v>3.3</v>
+      </c>
+      <c r="F7" s="2">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]), FagTabel[[#This Row],[ECTS-point]]*FagTabel[[#This Row],[Karakter]],"")</f>
         <v>75</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[ECTS karakter]]),FagTabel[[#This Row],[ECTS karakter]]*FagTabel[[#This Row],[ECTS-point]],"")</f>
+        <v>24.75</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <v>7.5</v>
       </c>
-      <c r="E8" s="4">
-        <f>IFERROR(FagTabel[[#This Row],[ECTS]]*FagTabel[[#This Row],[Karakter]], 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>12</v>
+      </c>
+      <c r="E8" s="2">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]),IF(D8=12,4,IF(D8=10,3.3,IF(D8=7,3,IF(D8=4,2.3,IF(D8=2,2,IF(D8=0,0,IF(D8=-3,0,"Ukendt karakter"))))))), "")</f>
+        <v>4</v>
+      </c>
+      <c r="F8" s="2">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]), FagTabel[[#This Row],[ECTS-point]]*FagTabel[[#This Row],[Karakter]],"")</f>
+        <v>90</v>
+      </c>
+      <c r="G8">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[ECTS karakter]]),FagTabel[[#This Row],[ECTS karakter]]*FagTabel[[#This Row],[ECTS-point]],"")</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9">
         <v>15</v>
       </c>
-      <c r="E9" s="4">
-        <f>IFERROR(FagTabel[[#This Row],[ECTS]]*FagTabel[[#This Row],[Karakter]], 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E9" s="2" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]),IF(D9=12,4,IF(D9=10,3.3,IF(D9=7,3,IF(D9=4,2.3,IF(D9=2,2,IF(D9=0,0,IF(D9=-3,0,"Ukendt karakter"))))))), "")</f>
+        <v/>
+      </c>
+      <c r="F9" s="2" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]), FagTabel[[#This Row],[ECTS-point]]*FagTabel[[#This Row],[Karakter]],"")</f>
+        <v/>
+      </c>
+      <c r="G9" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[ECTS karakter]]),FagTabel[[#This Row],[ECTS karakter]]*FagTabel[[#This Row],[ECTS-point]],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <v>15</v>
       </c>
-      <c r="E10" s="4">
-        <f>IFERROR(FagTabel[[#This Row],[ECTS]]*FagTabel[[#This Row],[Karakter]], 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E10" s="2" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]),IF(D10=12,4,IF(D10=10,3.3,IF(D10=7,3,IF(D10=4,2.3,IF(D10=2,2,IF(D10=0,0,IF(D10=-3,0,"Ukendt karakter"))))))), "")</f>
+        <v/>
+      </c>
+      <c r="F10" s="2" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]), FagTabel[[#This Row],[ECTS-point]]*FagTabel[[#This Row],[Karakter]],"")</f>
+        <v/>
+      </c>
+      <c r="G10" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[ECTS karakter]]),FagTabel[[#This Row],[ECTS karakter]]*FagTabel[[#This Row],[ECTS-point]],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11">
         <v>7.5</v>
       </c>
-      <c r="E11" s="4">
-        <f>IFERROR(FagTabel[[#This Row],[ECTS]]*FagTabel[[#This Row],[Karakter]], 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E11" s="2" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]),IF(D11=12,4,IF(D11=10,3.3,IF(D11=7,3,IF(D11=4,2.3,IF(D11=2,2,IF(D11=0,0,IF(D11=-3,0,"Ukendt karakter"))))))), "")</f>
+        <v/>
+      </c>
+      <c r="F11" s="2" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]), FagTabel[[#This Row],[ECTS-point]]*FagTabel[[#This Row],[Karakter]],"")</f>
+        <v/>
+      </c>
+      <c r="G11" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[ECTS karakter]]),FagTabel[[#This Row],[ECTS karakter]]*FagTabel[[#This Row],[ECTS-point]],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C12">
         <v>7.5</v>
       </c>
-      <c r="E12" s="4">
-        <f>IFERROR(FagTabel[[#This Row],[ECTS]]*FagTabel[[#This Row],[Karakter]], 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E12" s="2" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]),IF(D12=12,4,IF(D12=10,3.3,IF(D12=7,3,IF(D12=4,2.3,IF(D12=2,2,IF(D12=0,0,IF(D12=-3,0,"Ukendt karakter"))))))), "")</f>
+        <v/>
+      </c>
+      <c r="F12" s="2" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]), FagTabel[[#This Row],[ECTS-point]]*FagTabel[[#This Row],[Karakter]],"")</f>
+        <v/>
+      </c>
+      <c r="G12" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[ECTS karakter]]),FagTabel[[#This Row],[ECTS karakter]]*FagTabel[[#This Row],[ECTS-point]],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C13">
         <v>15</v>
       </c>
-      <c r="E13" s="4">
-        <f>IFERROR(FagTabel[[#This Row],[ECTS]]*FagTabel[[#This Row],[Karakter]], 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E13" s="2" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]),IF(D13=12,4,IF(D13=10,3.3,IF(D13=7,3,IF(D13=4,2.3,IF(D13=2,2,IF(D13=0,0,IF(D13=-3,0,"Ukendt karakter"))))))), "")</f>
+        <v/>
+      </c>
+      <c r="F13" s="2" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]), FagTabel[[#This Row],[ECTS-point]]*FagTabel[[#This Row],[Karakter]],"")</f>
+        <v/>
+      </c>
+      <c r="G13" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[ECTS karakter]]),FagTabel[[#This Row],[ECTS karakter]]*FagTabel[[#This Row],[ECTS-point]],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>15</v>
       </c>
-      <c r="E14" s="4">
-        <f>IFERROR(FagTabel[[#This Row],[ECTS]]*FagTabel[[#This Row],[Karakter]], 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E14" s="2" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]),IF(D14=12,4,IF(D14=10,3.3,IF(D14=7,3,IF(D14=4,2.3,IF(D14=2,2,IF(D14=0,0,IF(D14=-3,0,"Ukendt karakter"))))))), "")</f>
+        <v/>
+      </c>
+      <c r="F14" s="2" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]), FagTabel[[#This Row],[ECTS-point]]*FagTabel[[#This Row],[Karakter]],"")</f>
+        <v/>
+      </c>
+      <c r="G14" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[ECTS karakter]]),FagTabel[[#This Row],[ECTS karakter]]*FagTabel[[#This Row],[ECTS-point]],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C15">
         <v>7.5</v>
       </c>
-      <c r="E15" s="4">
-        <f>IFERROR(FagTabel[[#This Row],[ECTS]]*FagTabel[[#This Row],[Karakter]], 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E15" s="2" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]),IF(D15=12,4,IF(D15=10,3.3,IF(D15=7,3,IF(D15=4,2.3,IF(D15=2,2,IF(D15=0,0,IF(D15=-3,0,"Ukendt karakter"))))))), "")</f>
+        <v/>
+      </c>
+      <c r="F15" s="2" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]), FagTabel[[#This Row],[ECTS-point]]*FagTabel[[#This Row],[Karakter]],"")</f>
+        <v/>
+      </c>
+      <c r="G15" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[ECTS karakter]]),FagTabel[[#This Row],[ECTS karakter]]*FagTabel[[#This Row],[ECTS-point]],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C16">
         <v>7.5</v>
       </c>
-      <c r="E16" s="4">
-        <f>IFERROR(FagTabel[[#This Row],[ECTS]]*FagTabel[[#This Row],[Karakter]], 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E16" s="2" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]),IF(D16=12,4,IF(D16=10,3.3,IF(D16=7,3,IF(D16=4,2.3,IF(D16=2,2,IF(D16=0,0,IF(D16=-3,0,"Ukendt karakter"))))))), "")</f>
+        <v/>
+      </c>
+      <c r="F16" s="2" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]), FagTabel[[#This Row],[ECTS-point]]*FagTabel[[#This Row],[Karakter]],"")</f>
+        <v/>
+      </c>
+      <c r="G16" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[ECTS karakter]]),FagTabel[[#This Row],[ECTS karakter]]*FagTabel[[#This Row],[ECTS-point]],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C17">
         <v>15</v>
       </c>
-      <c r="E17">
-        <f>IFERROR(FagTabel[[#This Row],[ECTS]]*FagTabel[[#This Row],[Karakter]], 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="3">
-        <f>SUM(FagTabel[Vægtet karakter])</f>
-        <v>187.5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="6">
-        <f>SUMIF(FagTabel[Karakter], "&gt;0", FagTabel[ECTS])</f>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="9">
-        <f>C19/C20</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="10">
+      <c r="E17" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]),IF(D17=12,4,IF(D17=10,3.3,IF(D17=7,3,IF(D17=4,2.3,IF(D17=2,2,IF(D17=0,0,IF(D17=-3,0,"Ukendt karakter"))))))), "")</f>
+        <v/>
+      </c>
+      <c r="F17" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[Karakter]]), FagTabel[[#This Row],[ECTS-point]]*FagTabel[[#This Row],[Karakter]],"")</f>
+        <v/>
+      </c>
+      <c r="G17" t="str">
+        <f>IF(ISNUMBER(FagTabel[[#This Row],[ECTS karakter]]),FagTabel[[#This Row],[ECTS karakter]]*FagTabel[[#This Row],[ECTS-point]],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="7">
+        <f>SUMIF(FagTabel[Karakter],"&lt;&gt;", FagTabel[ECTS-point])</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="5">
+        <f>SUM(FagTabel[Vægtet karakter])/SUMIF(FagTabel[Karakter], "&gt;-4", FagTabel[ECTS-point])</f>
+        <v>6.166666666666667</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="6">
         <f>AVERAGEIF(FagTabel[Karakter], "&gt;-4")</f>
-        <v>5.75</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="5">
+        <f>SUM(FagTabel[ECTS-vægtet karakter])/SUMIF(FagTabel[ECTS karakter], "&gt;-4", FagTabel[ECTS-point])</f>
+        <v>2.7666666666666666</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="6">
+        <f>AVERAGEIF(FagTabel[ECTS karakter], "&gt;-4")</f>
+        <v>2.92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>